<commit_message>
pushing array and linkedlist changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/dsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/dsAlgo_TestData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishnaveniram/git/DSAlgo.RockStars/src/test/resources/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siris\git\DSAlgo.RockStars\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FDC136-C474-6A45-B738-632DFF6A1384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7681349B-65EB-44AD-8DFE-5931AB71D109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="22540" windowHeight="14300" activeTab="1" xr2:uid="{96C06443-7610-4BC9-9E10-3D39FD2144DD}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="2" xr2:uid="{96C06443-7610-4BC9-9E10-3D39FD2144DD}"/>
   </bookViews>
   <sheets>
     <sheet name="python code" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="dsalgocode" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
   <si>
     <t>output</t>
   </si>
@@ -150,6 +151,23 @@
   </si>
   <si>
     <t>You are logged in</t>
+  </si>
+  <si>
+    <t>print("Hello");</t>
+  </si>
+  <si>
+    <t>def search(input_list, num): 
+if(num in input_list):
+print("Element Found")
+\b
+\b
+else:
+print("Not Found")
+\b
+\b
+\b
+\b
+search([12, 23, 45, 67, 6, 90] , 12)</t>
   </si>
 </sst>
 </file>
@@ -261,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -273,6 +291,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,13 +612,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="88.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="88.6328125" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -607,7 +626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -615,13 +634,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -629,7 +648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -637,7 +656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -645,7 +664,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -653,7 +672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -661,7 +680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -669,7 +688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -677,7 +696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -694,18 +713,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181E224E-2837-0142-8AD8-569527ABC061}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
@@ -716,7 +735,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -727,7 +746,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>19</v>
       </c>
@@ -738,7 +757,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
@@ -749,7 +768,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>19</v>
       </c>
@@ -758,6 +777,111 @@
       </c>
       <c r="C5" s="7" t="s">
         <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9429FDAC-9F73-44C8-B623-9BE65DFF2AC9}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="195.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>